<commit_message>
code cleaned, comments added
</commit_message>
<xml_diff>
--- a/places_visited.xlsx
+++ b/places_visited.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lena\Desktop\pyladies\data_course\pyladies_vienna_data_course\streamlit_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D1D42D-7D46-4A62-AD40-B842495B73D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF00F36-3CCA-49A2-A594-2FE50C031BD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="184">
   <si>
     <t>place/city</t>
   </si>
@@ -564,9 +564,6 @@
   </si>
   <si>
     <t>home country</t>
-  </si>
-  <si>
-    <t>1977-</t>
   </si>
   <si>
     <t>St. Egyden am Steinfeld</t>
@@ -1449,7 +1446,7 @@
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>175</v>
@@ -2741,8 +2738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2774,9 +2771,6 @@
       <c r="B2" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>181</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -2969,7 +2963,7 @@
         <v>149</v>
       </c>
       <c r="B21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -2977,7 +2971,7 @@
         <v>151</v>
       </c>
       <c r="B22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
description moved above map, places loaded one after the other
</commit_message>
<xml_diff>
--- a/places_visited.xlsx
+++ b/places_visited.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lena\Desktop\pyladies\data_course\pyladies_vienna_data_course\streamlit_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC947E0-C365-4758-918E-E76D52EEF183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107CE7E1-B8EF-448C-83DF-128A007D86D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1427,13 +1427,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67:XFD67"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" customWidth="1"/>
+    <col min="1" max="1" width="30.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1977,7 +1977,7 @@
         <v>183</v>
       </c>
       <c r="B65" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>